<commit_message>
Some clean up and a lot of testing
</commit_message>
<xml_diff>
--- a/Interesting links.xlsx
+++ b/Interesting links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aurorahofman/Documents/Utveksling/Baysiana/UPC-Final-Project-Bayesian-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09428AA1-5D7C-1048-AAF7-BC69858EFF47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538FAF10-46FB-BF4C-8BAA-7CEE07ADAA29}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="12860" windowHeight="14740" xr2:uid="{C9875243-66A9-2A49-8908-43C8B46CDE86}"/>
   </bookViews>
@@ -616,7 +616,7 @@
   <dimension ref="A2:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>